<commit_message>
-Revive Phantom Knight 程式規格書.xlsx -Add Phantom Knight 美術、音樂、音效規格書.xlsx
</commit_message>
<xml_diff>
--- a/企劃/Phantom Knight 程式規格書.xlsx
+++ b/企劃/Phantom Knight 程式規格書.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="260">
   <si>
     <t>需求</t>
   </si>
@@ -192,6 +192,9 @@
     <t>。敵人AI</t>
   </si>
   <si>
+    <t>。音樂、音效</t>
+  </si>
+  <si>
     <t>。分數計算</t>
   </si>
   <si>
@@ -201,6 +204,12 @@
     <t>。遊戲暫停</t>
   </si>
   <si>
+    <t>。系統介面</t>
+  </si>
+  <si>
+    <t>。圖鑑、排行榜</t>
+  </si>
+  <si>
     <t>。獎勵</t>
   </si>
   <si>
@@ -232,6 +241,12 @@
   </si>
   <si>
     <t>。共有20波敵人(暫定)，理想上種類會比故事模式還多</t>
+  </si>
+  <si>
+    <t>流程圖參考：</t>
+  </si>
+  <si>
+    <t>https://app.diagrams.net/#G198RaeA3XA_b2Xfwl_2D2yFxYfitIzsvj</t>
   </si>
   <si>
     <t>產生敵人</t>
@@ -823,7 +838,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -873,6 +888,10 @@
       <color rgb="FF0000FF"/>
     </font>
     <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
@@ -907,7 +926,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -940,6 +959,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
@@ -965,7 +990,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1042,47 +1067,53 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="7" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1109,10 +1140,10 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4467225" cy="2514600"/>
+    <xdr:ext cx="4400550" cy="2476500"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="0" name="image1.png" title="圖片"/>
@@ -1120,6 +1151,62 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>-200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2733675" cy="5105400"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image3.png" title="圖片"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2905125</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2076450" cy="6457950"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image2.png" title="圖片"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1810,6 +1897,21 @@
         <v>50</v>
       </c>
     </row>
+    <row r="29">
+      <c r="C29" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C6"/>
@@ -1831,15 +1933,15 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="4.57"/>
     <col customWidth="1" min="2" max="2" width="24.71"/>
-    <col customWidth="1" min="3" max="3" width="41.43"/>
-    <col customWidth="1" min="4" max="4" width="53.43"/>
+    <col customWidth="1" min="3" max="3" width="43.43"/>
+    <col customWidth="1" min="4" max="4" width="58.43"/>
     <col customWidth="1" min="5" max="5" width="43.57"/>
   </cols>
   <sheetData>
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1866,253 +1968,267 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
+    <row r="3">
+      <c r="B3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="11"/>
+    </row>
     <row r="4">
-      <c r="B4" s="7" t="s">
-        <v>52</v>
+      <c r="B4" s="11" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="11" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="11" t="s">
-        <v>56</v>
-      </c>
+      <c r="B8" s="11"/>
     </row>
     <row r="9">
       <c r="B9" s="11"/>
     </row>
     <row r="10">
-      <c r="B10" s="11"/>
-    </row>
-    <row r="11">
-      <c r="B11" s="11" t="s">
-        <v>57</v>
+      <c r="B10" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="26">
-      <c r="B26" s="7" t="s">
-        <v>58</v>
+      <c r="B26" s="11" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" s="11" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" s="11" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="B31" s="11" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" s="30" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1"/>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1"/>
+      <c r="B38" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-      <c r="T33" s="1"/>
-      <c r="U33" s="1"/>
-      <c r="V33" s="1"/>
-      <c r="W33" s="1"/>
-      <c r="X33" s="1"/>
-      <c r="Y33" s="1"/>
-      <c r="Z33" s="1"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="6"/>
-      <c r="B34" s="7" t="s">
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+      <c r="Z38" s="1"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="6"/>
-      <c r="S34" s="6"/>
-      <c r="T34" s="6"/>
-      <c r="U34" s="6"/>
-      <c r="V34" s="6"/>
-      <c r="W34" s="6"/>
-      <c r="X34" s="6"/>
-      <c r="Y34" s="6"/>
-      <c r="Z34" s="6"/>
-    </row>
-    <row r="35">
-      <c r="B35" s="8" t="s">
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6"/>
+      <c r="R39" s="6"/>
+      <c r="S39" s="6"/>
+      <c r="T39" s="6"/>
+      <c r="U39" s="6"/>
+      <c r="V39" s="6"/>
+      <c r="W39" s="6"/>
+      <c r="X39" s="6"/>
+      <c r="Y39" s="6"/>
+      <c r="Z39" s="6"/>
+    </row>
+    <row r="40">
+      <c r="B40" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C40" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D40" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36">
-      <c r="B36" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E36" s="10"/>
-    </row>
-    <row r="37">
-      <c r="B37" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D37" s="9" t="s">
+    <row r="41">
+      <c r="B41" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E37" s="10"/>
-    </row>
-    <row r="38">
-      <c r="B38" s="9" t="s">
+      <c r="C41" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="D41" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-    </row>
-    <row r="39">
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-    </row>
-    <row r="40">
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
+      <c r="E41" s="10"/>
     </row>
     <row r="42">
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" s="10"/>
+    </row>
+    <row r="43">
+      <c r="B43" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+    </row>
+    <row r="44">
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+    </row>
+    <row r="45">
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+    </row>
+    <row r="47">
+      <c r="B47" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43">
-      <c r="B43" s="12" t="s">
+    <row r="48">
+      <c r="B48" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C48" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D48" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="44">
-      <c r="B44" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="B45" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="B46" s="9" t="s">
+    <row r="49">
+      <c r="B49" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C49" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D49" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="47">
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-    </row>
-    <row r="48">
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
+    <row r="50">
+      <c r="B50" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+    </row>
+    <row r="53">
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" location="G198RaeA3XA_b2Xfwl_2D2yFxYfitIzsvj" ref="B33"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2136,7 +2252,7 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2165,88 +2281,88 @@
     </row>
     <row r="3">
       <c r="B3" s="11" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>81</v>
+      <c r="B5" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="9" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="9" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="9" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="9" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="9" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="7" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="11" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="11" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15">
@@ -2257,27 +2373,27 @@
     </row>
     <row r="17">
       <c r="B17" s="7" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="11" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="11" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="11" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="31" t="s">
-        <v>102</v>
+      <c r="B21" s="33" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="22">
@@ -2285,145 +2401,145 @@
     </row>
     <row r="23">
       <c r="B23" s="11" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="11" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" s="11" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" s="7" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" s="11" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="11" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31">
-      <c r="B31" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="D31" s="33" t="s">
-        <v>109</v>
+      <c r="B31" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" s="11" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" s="11" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" s="11" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" s="11" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" s="7" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" s="11" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" s="11" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" s="11" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" s="11" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" s="7" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" s="11" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" s="11" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" s="11" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" s="11" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" s="11" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" s="11" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" s="11" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" s="11" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" s="11" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" s="11" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" s="11" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60">
@@ -2481,78 +2597,78 @@
     </row>
     <row r="63">
       <c r="B63" s="9" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E63" s="10"/>
     </row>
     <row r="64">
       <c r="B64" s="9" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="E64" s="33" t="s">
-        <v>109</v>
+        <v>138</v>
+      </c>
+      <c r="E64" s="35" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" s="9" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D65" s="10"/>
       <c r="E65" s="10"/>
     </row>
     <row r="66">
       <c r="B66" s="9" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E66" s="10"/>
     </row>
     <row r="67">
       <c r="B67" s="9" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D67" s="10"/>
       <c r="E67" s="10"/>
     </row>
     <row r="68">
       <c r="B68" s="9" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D68" s="10"/>
       <c r="E68" s="10"/>
     </row>
     <row r="69">
       <c r="B69" s="9" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D69" s="10"/>
       <c r="E69" s="10"/>
@@ -2578,80 +2694,80 @@
     </row>
     <row r="74">
       <c r="B74" s="14" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="75">
       <c r="B75" s="9" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="76">
       <c r="B76" s="9" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D76" s="10"/>
     </row>
     <row r="77">
       <c r="B77" s="9" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D77" s="10"/>
     </row>
     <row r="78">
       <c r="B78" s="9" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D78" s="10"/>
     </row>
     <row r="79">
       <c r="B79" s="9" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D79" s="10"/>
     </row>
     <row r="80">
       <c r="B80" s="9" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D80" s="10"/>
     </row>
     <row r="81">
       <c r="B81" s="14" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D81" s="16" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2684,7 +2800,7 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2713,77 +2829,77 @@
     </row>
     <row r="3">
       <c r="B3" s="11" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="31" t="s">
-        <v>157</v>
+      <c r="B4" s="33" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="31"/>
+      <c r="B5" s="33"/>
     </row>
     <row r="6">
       <c r="B6" s="7" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7">
       <c r="B7" s="9" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="D7" s="10"/>
     </row>
     <row r="8">
       <c r="B8" s="9" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="D8" s="10"/>
     </row>
     <row r="9">
       <c r="B9" s="9" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10">
       <c r="B10" s="9" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="D10" s="10"/>
     </row>
     <row r="11">
       <c r="B11" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>168</v>
+        <v>172</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>173</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="9" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="D12" s="10"/>
     </row>
@@ -2794,100 +2910,100 @@
     </row>
     <row r="15">
       <c r="B15" s="7" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="9" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="9" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="9" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="9" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="9" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" s="9" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="7" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" s="9" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="D25" s="10"/>
     </row>
@@ -2999,179 +3115,179 @@
       </c>
     </row>
     <row r="42">
-      <c r="B42" s="35" t="s">
+      <c r="B42" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C42" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="36" t="s">
+      <c r="D42" s="38" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="43">
-      <c r="B43" s="37" t="s">
-        <v>159</v>
-      </c>
-      <c r="C43" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="D43" s="38"/>
+      <c r="B43" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="C43" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="40"/>
     </row>
     <row r="44">
-      <c r="B44" s="39" t="s">
-        <v>161</v>
-      </c>
-      <c r="C44" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="D44" s="40"/>
+      <c r="B44" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="C44" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="42"/>
     </row>
     <row r="45">
-      <c r="B45" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="C45" s="39" t="s">
-        <v>70</v>
-      </c>
-      <c r="D45" s="39"/>
+      <c r="B45" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="C45" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" s="41"/>
     </row>
     <row r="46">
-      <c r="B46" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="C46" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D46" s="39" t="s">
-        <v>198</v>
+      <c r="B46" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="C46" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" s="41" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="47">
-      <c r="B47" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="C47" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D47" s="39" t="s">
-        <v>199</v>
+      <c r="B47" s="41" t="s">
+        <v>172</v>
+      </c>
+      <c r="C47" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" s="41" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="48">
-      <c r="B48" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="C48" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D48" s="39" t="s">
-        <v>200</v>
+      <c r="B48" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="C48" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="41" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="49">
-      <c r="B49" s="41" t="s">
-        <v>201</v>
-      </c>
-      <c r="C49" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D49" s="39" t="s">
-        <v>202</v>
+      <c r="B49" s="43" t="s">
+        <v>206</v>
+      </c>
+      <c r="C49" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="41" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="50">
-      <c r="B50" s="41" t="s">
+      <c r="B50" s="43" t="s">
+        <v>208</v>
+      </c>
+      <c r="C50" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" s="41" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" s="39" t="s">
+        <v>209</v>
+      </c>
+      <c r="C51" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="39" t="s">
         <v>203</v>
       </c>
-      <c r="C50" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D50" s="39" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="B51" s="37" t="s">
-        <v>204</v>
-      </c>
-      <c r="C51" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D51" s="37" t="s">
-        <v>198</v>
-      </c>
     </row>
     <row r="52">
-      <c r="B52" s="37" t="s">
-        <v>205</v>
-      </c>
-      <c r="C52" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D52" s="37" t="s">
-        <v>202</v>
+      <c r="B52" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="C52" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="39" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="53">
-      <c r="B53" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="C53" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D53" s="37" t="s">
-        <v>198</v>
+      <c r="B53" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="C53" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D53" s="39" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="54">
-      <c r="B54" s="41" t="s">
+      <c r="B54" s="43" t="s">
+        <v>212</v>
+      </c>
+      <c r="C54" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D54" s="41" t="s">
         <v>207</v>
       </c>
-      <c r="C54" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D54" s="39" t="s">
-        <v>202</v>
-      </c>
     </row>
     <row r="55">
-      <c r="B55" s="41" t="s">
-        <v>208</v>
-      </c>
-      <c r="C55" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D55" s="37" t="s">
-        <v>198</v>
+      <c r="B55" s="43" t="s">
+        <v>213</v>
+      </c>
+      <c r="C55" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" s="39" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="56">
-      <c r="B56" s="41" t="s">
-        <v>209</v>
-      </c>
-      <c r="C56" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D56" s="39" t="s">
-        <v>202</v>
+      <c r="B56" s="43" t="s">
+        <v>214</v>
+      </c>
+      <c r="C56" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D56" s="41" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="57">
-      <c r="B57" s="41" t="s">
-        <v>210</v>
-      </c>
-      <c r="C57" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D57" s="37" t="s">
-        <v>198</v>
+      <c r="B57" s="43" t="s">
+        <v>215</v>
+      </c>
+      <c r="C57" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D57" s="39" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="58">
-      <c r="B58" s="41"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="37"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="39"/>
     </row>
   </sheetData>
   <drawing r:id="rId2"/>
@@ -3199,7 +3315,7 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3228,85 +3344,85 @@
     </row>
     <row r="4">
       <c r="B4" s="7" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="9" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="D5" s="42"/>
+        <v>220</v>
+      </c>
+      <c r="D5" s="44"/>
     </row>
     <row r="6">
       <c r="B6" s="9" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="9" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="D7" s="10"/>
     </row>
     <row r="8">
       <c r="B8" s="9" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="D8" s="10"/>
     </row>
     <row r="9">
       <c r="B9" s="9" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10">
       <c r="B10" s="9" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="D10" s="10"/>
     </row>
     <row r="11">
       <c r="B11" s="9" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="9" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="D12" s="10"/>
     </row>
@@ -3317,32 +3433,32 @@
     </row>
     <row r="15">
       <c r="B15" s="7" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="11" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="11" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="11" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="11" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="11" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24">
@@ -3443,120 +3559,120 @@
       <c r="B34" s="11"/>
     </row>
     <row r="36">
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
     </row>
     <row r="37">
-      <c r="B37" s="35" t="s">
+      <c r="B37" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="36" t="s">
+      <c r="D37" s="38" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="38">
-      <c r="B38" s="37" t="s">
-        <v>238</v>
-      </c>
-      <c r="C38" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="D38" s="37" t="s">
-        <v>239</v>
+      <c r="B38" s="39" t="s">
+        <v>243</v>
+      </c>
+      <c r="C38" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="39" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="39">
-      <c r="B39" s="37" t="s">
-        <v>240</v>
-      </c>
-      <c r="C39" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="D39" s="37" t="s">
-        <v>241</v>
+      <c r="B39" s="39" t="s">
+        <v>245</v>
+      </c>
+      <c r="C39" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="39" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="40">
-      <c r="B40" s="37" t="s">
-        <v>242</v>
-      </c>
-      <c r="C40" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="D40" s="37" t="s">
-        <v>243</v>
+      <c r="B40" s="39" t="s">
+        <v>247</v>
+      </c>
+      <c r="C40" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="39" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="41">
-      <c r="B41" s="37" t="s">
-        <v>244</v>
-      </c>
-      <c r="C41" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="D41" s="37" t="s">
-        <v>245</v>
+      <c r="B41" s="39" t="s">
+        <v>249</v>
+      </c>
+      <c r="C41" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="39" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" s="9" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" s="9" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" s="9" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" s="9" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" s="9" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47">

</xml_diff>

<commit_message>
- Phantom Knight 程式規格書.xlsx alpha 1.1
</commit_message>
<xml_diff>
--- a/企劃/Phantom Knight 程式規格書.xlsx
+++ b/企劃/Phantom Knight 程式規格書.xlsx
@@ -9,7 +9,8 @@
     <sheet state="visible" name="基本玩法" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="操作" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="角色數值、狀態" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="道具與桑丘" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="效果觸發" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="道具與桑丘" sheetId="8" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -22,7 +23,23 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="B46">
+    <comment authorId="0" ref="B63">
+      <text>
+        <t xml:space="preserve">可多加一列『按鍵方法』
+	-Henry Kuh
+是指鍵位嗎
+	-Bridge Lin</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B49">
+      <text>
+        <t xml:space="preserve">BOSS 可以抓嗎？
+	-Bogay Chuang
+我是想不行
+	-Bridge Lin</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B47">
       <text>
         <t xml:space="preserve">這個功能感覺比較難做，可能需要討論一下。
 	-Bridge Lin</t>
@@ -38,6 +55,28 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="C15">
+      <text>
+        <t xml:space="preserve">疊加的方式，加還是乘
+	-Bridge Lin
+Bogay：可是可以疊加
+喔還有 buff 的疊加
+是用乘的還是加的
+那 +10% &amp; -10% 同時出現
+結果是 99% 還是 100%
+邏輯上有點不同
+	-Bridge Lin</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C9">
+      <text>
+        <t xml:space="preserve">一點擋一次？不論傷害高低嗎？
+擋狀態是指什麼？帶狀態效果的攻擊需要消耗兩點的意思？哪個比較優先？
+	-Bogay Chuang
+改成不能擋狀態好了，這點我之前沒想清楚QAQ
+	-Bridge Lin</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="D22">
       <text>
         <t xml:space="preserve">獎勵可能放在三、、四級製作目標，有一些強力Build也有對應抑制的效果
@@ -48,8 +87,26 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="B15">
+      <text>
+        <t xml:space="preserve">必殺技聽起來像是三級製作目標 XD
+	-Henry Kuh
+對XDDD
+	-Bridge Lin</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="270">
   <si>
     <t>需求</t>
   </si>
@@ -99,6 +156,12 @@
     <t>建立本表</t>
   </si>
   <si>
+    <t>Alpha1.1</t>
+  </si>
+  <si>
+    <t>依照開會內容修改概要、操作、角色數值狀態。</t>
+  </si>
+  <si>
     <t>概要</t>
   </si>
   <si>
@@ -174,6 +237,9 @@
     <t>功能概要</t>
   </si>
   <si>
+    <t>一級、二級(優先製作)</t>
+  </si>
+  <si>
     <t>。基本玩法</t>
   </si>
   <si>
@@ -183,30 +249,36 @@
     <t>。角色數值、狀態</t>
   </si>
   <si>
+    <t>。戰鬥判定</t>
+  </si>
+  <si>
+    <t>。敵人AI</t>
+  </si>
+  <si>
+    <t>。場景</t>
+  </si>
+  <si>
+    <t>。分數計算</t>
+  </si>
+  <si>
+    <t>。系統介面</t>
+  </si>
+  <si>
+    <t>。音樂、音效的控制</t>
+  </si>
+  <si>
+    <t>。遊戲暫停</t>
+  </si>
+  <si>
+    <t>三級</t>
+  </si>
+  <si>
+    <t>。效果觸發</t>
+  </si>
+  <si>
     <t>。道具與桑丘</t>
   </si>
   <si>
-    <t>。戰鬥判定</t>
-  </si>
-  <si>
-    <t>。敵人AI</t>
-  </si>
-  <si>
-    <t>。音樂、音效</t>
-  </si>
-  <si>
-    <t>。分數計算</t>
-  </si>
-  <si>
-    <t>。場景</t>
-  </si>
-  <si>
-    <t>。遊戲暫停</t>
-  </si>
-  <si>
-    <t>。系統介面</t>
-  </si>
-  <si>
     <t>。圖鑑、排行榜</t>
   </si>
   <si>
@@ -297,12 +369,36 @@
     <t>記錄戰鬥進行多久</t>
   </si>
   <si>
-    <t>操作</t>
+    <t>一級目標</t>
   </si>
   <si>
     <t>本作的操作有移動、普攻、跳躍、翻滾、使用道具五種</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FFFF0000"/>
+      </rPr>
+      <t>三級製作目標：每一個操作都能觸發相對應的特效，詳見</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </rPr>
+      <t>效果觸發</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FFFF0000"/>
+      </rPr>
+      <t>的分頁</t>
+    </r>
+  </si>
+  <si>
     <t>鍵位</t>
   </si>
   <si>
@@ -375,15 +471,9 @@
     <t>不自帶擊退效果</t>
   </si>
   <si>
-    <t>許願：</t>
-  </si>
-  <si>
     <t>三段連段：類似死亡細胞、黑帝斯那樣連續按攻擊會有不同的動畫與特效，且傷害也不同</t>
   </si>
   <si>
-    <t>觸發普攻特殊效果：若有獎勵技能可以在普攻上放置特殊效果，使用時觸發(例如：普攻造成暈眩等)</t>
-  </si>
-  <si>
     <t>有慣性的跳躍</t>
   </si>
   <si>
@@ -423,7 +513,7 @@
     <t>抓住最近的角色，再按一下將其拋出</t>
   </si>
   <si>
-    <t>若是敵人血量必須低於其可抓/拋比率</t>
+    <t>敵人血量低於其可抓/拋比率才可抓</t>
   </si>
   <si>
     <t>播放抓/拋動畫</t>
@@ -453,6 +543,12 @@
     <t>拋擲的攻擊力加成</t>
   </si>
   <si>
+    <t>按鍵</t>
+  </si>
+  <si>
+    <t>獲取來自手把、鍵鼠的訊號</t>
+  </si>
+  <si>
     <t>左右移動</t>
   </si>
   <si>
@@ -552,13 +648,13 @@
     <t>血量</t>
   </si>
   <si>
-    <t>點數，玩家角色血量歸零則遊戲結束，敵人血量歸零則死亡</t>
+    <t>點數，玩家角色血量歸零則遊戲結束，敵人血量歸零則觸發死亡效果</t>
   </si>
   <si>
     <t>護盾</t>
   </si>
   <si>
-    <t>一點可以擋掉一次攻擊的傷害與來自敵人的狀態</t>
+    <t>一點可以擋掉一次攻擊的傷害(無論大小)</t>
   </si>
   <si>
     <t>攻擊速度</t>
@@ -582,6 +678,15 @@
     <t>百分比，血量在此比率下的敵人可被抓拋</t>
   </si>
   <si>
+    <t>硬直</t>
+  </si>
+  <si>
+    <t>受到傷害時，播放受傷動畫，不能攻擊與移動</t>
+  </si>
+  <si>
+    <t>(玩家)硬直時不會受到傷害</t>
+  </si>
+  <si>
     <t>狀態</t>
   </si>
   <si>
@@ -669,10 +774,13 @@
     <t>百分比</t>
   </si>
   <si>
+    <t>硬直時間</t>
+  </si>
+  <si>
+    <t>秒</t>
+  </si>
+  <si>
     <t>暈眩時間</t>
-  </si>
-  <si>
-    <t>秒</t>
   </si>
   <si>
     <t>無敵時間</t>
@@ -838,7 +946,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -912,6 +1020,11 @@
     <font>
       <sz val="10.0"/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -990,7 +1103,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="53">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1044,8 +1157,8 @@
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -1067,27 +1180,40 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf borderId="0" fillId="7" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -1106,11 +1232,14 @@
     <xf borderId="1" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="7" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyFont="1"/>
@@ -1232,6 +1361,10 @@
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1652,7 +1785,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="47.29"/>
+    <col customWidth="1" min="4" max="4" width="84.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1684,10 +1817,18 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
+      <c r="A3" s="19">
+        <v>44636.0</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1710,7 +1851,7 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1739,7 +1880,7 @@
     </row>
     <row r="3">
       <c r="B3" s="22" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" s="23"/>
     </row>
@@ -1749,50 +1890,50 @@
     </row>
     <row r="5">
       <c r="B5" s="25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="27" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="27" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="27" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="27" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
@@ -1800,42 +1941,42 @@
     </row>
     <row r="12">
       <c r="B12" s="27" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="27" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="27" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="27" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17">
@@ -1844,72 +1985,91 @@
     </row>
     <row r="18">
       <c r="B18" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19">
-      <c r="C19" s="11" t="s">
-        <v>41</v>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="20">
       <c r="C20" s="11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21">
       <c r="C21" s="11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22">
       <c r="C22" s="11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23">
       <c r="C23" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24">
       <c r="C24" s="11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25">
       <c r="C25" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26">
       <c r="C26" s="11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27">
       <c r="C27" s="11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28">
       <c r="C28" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29">
       <c r="C29" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30">
-      <c r="C30" s="11" t="s">
-        <v>52</v>
-      </c>
+      <c r="C30" s="7"/>
     </row>
     <row r="31">
-      <c r="C31" s="11" t="s">
-        <v>53</v>
+      <c r="C31" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" s="30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="C33" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="C34" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="C35" s="11" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1941,7 +2101,7 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1970,28 +2130,28 @@
     </row>
     <row r="3">
       <c r="B3" s="7" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D3" s="11"/>
     </row>
     <row r="4">
       <c r="B4" s="11" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="11" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="11" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8">
@@ -2002,47 +2162,47 @@
     </row>
     <row r="10">
       <c r="B10" s="11" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" s="7" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="11" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" s="11" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" s="11" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="11" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="30" t="s">
-        <v>64</v>
+      <c r="B32" s="31" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="33">
-      <c r="B33" s="31" t="s">
-        <v>65</v>
+      <c r="B33" s="32" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="38">
@@ -2121,34 +2281,34 @@
     </row>
     <row r="41">
       <c r="B41" s="9" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E41" s="10"/>
     </row>
     <row r="42">
       <c r="B42" s="9" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E42" s="10"/>
     </row>
     <row r="43">
       <c r="B43" s="9" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
@@ -2183,35 +2343,35 @@
     </row>
     <row r="49">
       <c r="B49" s="9" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" s="9" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" s="9" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52">
@@ -2252,7 +2412,7 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2281,499 +2441,526 @@
     </row>
     <row r="3">
       <c r="B3" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="33" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>89</v>
+      <c r="B6" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="9" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="9" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="9" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="7" t="s">
-        <v>87</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="11" t="s">
-        <v>102</v>
+      <c r="B13" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="11" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="11"/>
+      <c r="B15" s="11" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="16">
       <c r="B16" s="11"/>
     </row>
     <row r="17">
-      <c r="B17" s="7" t="s">
-        <v>90</v>
-      </c>
+      <c r="B17" s="11"/>
     </row>
     <row r="18">
-      <c r="B18" s="11" t="s">
-        <v>104</v>
+      <c r="B18" s="7" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="11" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="11" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="33" t="s">
-        <v>107</v>
+      <c r="B21" s="11" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="11"/>
+      <c r="B22" s="33" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="23">
       <c r="B23" s="11" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" s="7" t="s">
-        <v>93</v>
-      </c>
+      <c r="B24" s="11"/>
     </row>
     <row r="29">
-      <c r="B29" s="11" t="s">
-        <v>111</v>
+      <c r="B29" s="7" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="11" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31">
-      <c r="B31" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="D31" s="35" t="s">
-        <v>114</v>
+      <c r="B31" s="11" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="11" t="s">
-        <v>115</v>
+      <c r="B32" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D32" s="36" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" s="11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="B35" s="11" t="s">
-        <v>117</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" s="11" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="B38" s="7" t="s">
-        <v>96</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" s="11" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="39">
-      <c r="B39" s="11" t="s">
-        <v>119</v>
+      <c r="B39" s="7" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" s="11" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="B43" s="11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="B46" s="7" t="s">
-        <v>99</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" s="11" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="47">
-      <c r="B47" s="11" t="s">
-        <v>123</v>
+      <c r="B47" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" s="11" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" s="11" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" s="11" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" s="11" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" s="11" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" s="11" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" s="11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="B56" s="11" t="s">
-        <v>131</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" s="11" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" s="11" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" s="11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1"/>
-      <c r="B60" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1"/>
+      <c r="B61" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="5"/>
-      <c r="K60" s="5"/>
-      <c r="L60" s="5"/>
-      <c r="M60" s="5"/>
-      <c r="N60" s="5"/>
-      <c r="O60" s="5"/>
-      <c r="P60" s="5"/>
-      <c r="Q60" s="5"/>
-      <c r="R60" s="5"/>
-      <c r="S60" s="5"/>
-      <c r="T60" s="5"/>
-      <c r="U60" s="5"/>
-      <c r="V60" s="5"/>
-      <c r="W60" s="5"/>
-      <c r="X60" s="5"/>
-      <c r="Y60" s="5"/>
-      <c r="Z60" s="5"/>
-    </row>
-    <row r="61">
-      <c r="A61" s="6"/>
-      <c r="B61" s="7" t="s">
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="5"/>
+      <c r="O61" s="5"/>
+      <c r="P61" s="5"/>
+      <c r="Q61" s="5"/>
+      <c r="R61" s="5"/>
+      <c r="S61" s="5"/>
+      <c r="T61" s="5"/>
+      <c r="U61" s="5"/>
+      <c r="V61" s="5"/>
+      <c r="W61" s="5"/>
+      <c r="X61" s="5"/>
+      <c r="Y61" s="5"/>
+      <c r="Z61" s="5"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="6"/>
+      <c r="B62" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6"/>
-    </row>
-    <row r="62">
-      <c r="B62" s="8" t="s">
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+    </row>
+    <row r="63">
+      <c r="B63" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="C63" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="D63" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="E63" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="63">
-      <c r="B63" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="E63" s="10"/>
-    </row>
     <row r="64">
-      <c r="B64" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="D64" s="9" t="s">
+      <c r="A64" s="37"/>
+      <c r="B64" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="E64" s="35" t="s">
-        <v>114</v>
-      </c>
+      <c r="C64" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="37"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="37"/>
+      <c r="I64" s="37"/>
+      <c r="J64" s="37"/>
+      <c r="K64" s="37"/>
+      <c r="L64" s="37"/>
+      <c r="M64" s="37"/>
+      <c r="N64" s="37"/>
+      <c r="O64" s="37"/>
+      <c r="P64" s="37"/>
+      <c r="Q64" s="37"/>
+      <c r="R64" s="37"/>
+      <c r="S64" s="37"/>
+      <c r="T64" s="37"/>
+      <c r="U64" s="37"/>
+      <c r="V64" s="37"/>
+      <c r="W64" s="37"/>
+      <c r="X64" s="37"/>
+      <c r="Y64" s="37"/>
+      <c r="Z64" s="37"/>
     </row>
     <row r="65">
       <c r="B65" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="D65" s="10"/>
+        <v>141</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="E65" s="10"/>
     </row>
     <row r="66">
       <c r="B66" s="9" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="E66" s="10"/>
+        <v>144</v>
+      </c>
+      <c r="E66" s="36" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="67">
       <c r="B67" s="9" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D67" s="10"/>
       <c r="E67" s="10"/>
     </row>
     <row r="68">
       <c r="B68" s="9" t="s">
-        <v>145</v>
+        <v>102</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="D68" s="10"/>
+        <v>147</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>148</v>
+      </c>
       <c r="E68" s="10"/>
     </row>
     <row r="69">
       <c r="B69" s="9" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D69" s="10"/>
       <c r="E69" s="10"/>
     </row>
     <row r="70">
-      <c r="B70" s="11"/>
+      <c r="B70" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+    </row>
+    <row r="71">
+      <c r="B71" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
     </row>
     <row r="72">
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="11"/>
+    </row>
+    <row r="74">
+      <c r="B74" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="73">
-      <c r="B73" s="12" t="s">
+    <row r="75">
+      <c r="B75" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C73" s="13" t="s">
+      <c r="C75" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D73" s="13" t="s">
+      <c r="D75" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="74">
-      <c r="B74" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="C74" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="D74" s="14" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="B75" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D75" s="9" t="s">
-        <v>152</v>
-      </c>
-    </row>
     <row r="76">
-      <c r="B76" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D76" s="10"/>
+      <c r="B76" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="77">
       <c r="B77" s="9" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D77" s="10"/>
+        <v>85</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="78">
       <c r="B78" s="9" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D78" s="10"/>
     </row>
     <row r="79">
       <c r="B79" s="9" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D79" s="10"/>
     </row>
     <row r="80">
       <c r="B80" s="9" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D80" s="10"/>
     </row>
     <row r="81">
-      <c r="B81" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="C81" s="14" t="s">
+      <c r="B81" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D81" s="10"/>
+    </row>
+    <row r="82">
+      <c r="B82" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C82" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D81" s="16" t="s">
-        <v>159</v>
+      <c r="D82" s="10"/>
+    </row>
+    <row r="83">
+      <c r="B83" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D83" s="16" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="D31"/>
-    <hyperlink r:id="rId3" ref="E64"/>
+    <hyperlink r:id="rId2" ref="D32"/>
+    <hyperlink r:id="rId3" ref="E66"/>
   </hyperlinks>
   <drawing r:id="rId4"/>
   <legacyDrawing r:id="rId5"/>
@@ -2792,7 +2979,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="5.43"/>
     <col customWidth="1" min="2" max="2" width="14.29"/>
-    <col customWidth="1" min="3" max="3" width="53.43"/>
+    <col customWidth="1" min="3" max="3" width="61.43"/>
     <col customWidth="1" min="4" max="4" width="70.0"/>
     <col customWidth="1" min="5" max="5" width="43.29"/>
   </cols>
@@ -2800,7 +2987,7 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2829,12 +3016,12 @@
     </row>
     <row r="3">
       <c r="B3" s="11" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="33" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5">
@@ -2842,168 +3029,174 @@
     </row>
     <row r="6">
       <c r="B6" s="7" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7">
       <c r="B7" s="9" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="D7" s="10"/>
     </row>
     <row r="8">
       <c r="B8" s="9" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D8" s="10"/>
     </row>
     <row r="9">
       <c r="B9" s="9" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10">
       <c r="B10" s="9" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D10" s="10"/>
     </row>
     <row r="11">
       <c r="B11" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>173</v>
+        <v>178</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>179</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="9" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="D12" s="10"/>
     </row>
     <row r="13">
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
+      <c r="B13" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" s="7" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="9" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="9" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="9" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="9" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="9" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="9" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" s="9" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="7" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" s="9" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="D25" s="10"/>
     </row>
@@ -3115,179 +3308,190 @@
       </c>
     </row>
     <row r="42">
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="38" t="s">
+      <c r="C42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="38" t="s">
+      <c r="D42" s="43" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="43">
-      <c r="B43" s="39" t="s">
-        <v>164</v>
-      </c>
-      <c r="C43" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D43" s="40"/>
+      <c r="B43" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="C43" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="45"/>
     </row>
     <row r="44">
-      <c r="B44" s="41" t="s">
-        <v>166</v>
-      </c>
-      <c r="C44" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D44" s="42"/>
+      <c r="B44" s="46" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="47"/>
     </row>
     <row r="45">
-      <c r="B45" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="C45" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="D45" s="41"/>
+      <c r="B45" s="46" t="s">
+        <v>174</v>
+      </c>
+      <c r="C45" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="46"/>
     </row>
     <row r="46">
-      <c r="B46" s="41" t="s">
-        <v>170</v>
-      </c>
-      <c r="C46" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="D46" s="41" t="s">
-        <v>203</v>
+      <c r="B46" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="C46" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="D46" s="46" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="47">
-      <c r="B47" s="41" t="s">
-        <v>172</v>
-      </c>
-      <c r="C47" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="D47" s="41" t="s">
-        <v>204</v>
+      <c r="B47" s="46" t="s">
+        <v>178</v>
+      </c>
+      <c r="C47" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" s="46" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="48">
-      <c r="B48" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="C48" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="D48" s="41" t="s">
-        <v>205</v>
+      <c r="B48" s="46" t="s">
+        <v>181</v>
+      </c>
+      <c r="C48" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" s="46" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="49">
-      <c r="B49" s="43" t="s">
-        <v>206</v>
-      </c>
-      <c r="C49" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="D49" s="41" t="s">
-        <v>207</v>
+      <c r="B49" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="C49" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D49" s="48" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="50">
-      <c r="B50" s="43" t="s">
-        <v>208</v>
-      </c>
-      <c r="C50" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="D50" s="41" t="s">
-        <v>207</v>
+      <c r="B50" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="C50" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="D50" s="46" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="51">
-      <c r="B51" s="39" t="s">
-        <v>209</v>
-      </c>
-      <c r="C51" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="D51" s="39" t="s">
-        <v>203</v>
+      <c r="B51" s="49" t="s">
+        <v>218</v>
+      </c>
+      <c r="C51" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51" s="46" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="52">
-      <c r="B52" s="39" t="s">
-        <v>210</v>
-      </c>
-      <c r="C52" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="D52" s="39" t="s">
-        <v>207</v>
+      <c r="B52" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="C52" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="D52" s="44" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="53">
-      <c r="B53" s="39" t="s">
-        <v>211</v>
-      </c>
-      <c r="C53" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="D53" s="39" t="s">
-        <v>203</v>
+      <c r="B53" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C53" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="D53" s="44" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="54">
-      <c r="B54" s="43" t="s">
+      <c r="B54" s="44" t="s">
+        <v>221</v>
+      </c>
+      <c r="C54" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54" s="44" t="s">
         <v>212</v>
       </c>
-      <c r="C54" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="D54" s="41" t="s">
-        <v>207</v>
-      </c>
     </row>
     <row r="55">
-      <c r="B55" s="43" t="s">
-        <v>213</v>
-      </c>
-      <c r="C55" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="D55" s="39" t="s">
-        <v>203</v>
+      <c r="B55" s="49" t="s">
+        <v>222</v>
+      </c>
+      <c r="C55" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55" s="46" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="56">
-      <c r="B56" s="43" t="s">
-        <v>214</v>
-      </c>
-      <c r="C56" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="D56" s="41" t="s">
-        <v>207</v>
+      <c r="B56" s="49" t="s">
+        <v>223</v>
+      </c>
+      <c r="C56" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="D56" s="44" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="57">
-      <c r="B57" s="43" t="s">
-        <v>215</v>
-      </c>
-      <c r="C57" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="D57" s="39" t="s">
-        <v>203</v>
+      <c r="B57" s="49" t="s">
+        <v>224</v>
+      </c>
+      <c r="C57" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="D57" s="46" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="58">
-      <c r="B58" s="43"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="39"/>
+      <c r="B58" s="49" t="s">
+        <v>225</v>
+      </c>
+      <c r="C58" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="D58" s="44" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" s="49"/>
+      <c r="C59" s="45"/>
+      <c r="D59" s="44"/>
     </row>
   </sheetData>
   <drawing r:id="rId2"/>
@@ -3306,17 +3510,15 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="5.43"/>
-    <col customWidth="1" min="2" max="2" width="18.29"/>
-    <col customWidth="1" min="3" max="3" width="62.43"/>
-    <col customWidth="1" min="4" max="4" width="59.86"/>
+    <col customWidth="1" min="2" max="2" width="14.29"/>
+    <col customWidth="1" min="3" max="3" width="44.71"/>
+    <col customWidth="1" min="4" max="4" width="49.71"/>
     <col customWidth="1" min="5" max="5" width="43.29"/>
   </cols>
   <sheetData>
     <row r="2">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
-        <v>216</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -3342,87 +3544,302 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
+    <row r="5">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="1"/>
+      <c r="B18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28">
+      <c r="B28" s="11"/>
+    </row>
+    <row r="30">
+      <c r="B30" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+    </row>
+    <row r="33">
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+    </row>
+    <row r="34">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="10"/>
+    </row>
+    <row r="36">
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="10"/>
+    </row>
+    <row r="37">
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="10"/>
+    </row>
+    <row r="38">
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="10"/>
+    </row>
+    <row r="39">
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="10"/>
+    </row>
+    <row r="40">
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="16"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="5.43"/>
+    <col customWidth="1" min="2" max="2" width="18.29"/>
+    <col customWidth="1" min="3" max="3" width="62.43"/>
+    <col customWidth="1" min="4" max="4" width="59.86"/>
+    <col customWidth="1" min="5" max="5" width="43.29"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+    </row>
     <row r="4">
       <c r="B4" s="7" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="9" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="D5" s="44"/>
+        <v>230</v>
+      </c>
+      <c r="D5" s="50"/>
     </row>
     <row r="6">
       <c r="B6" s="9" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="9" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="D7" s="10"/>
     </row>
     <row r="8">
       <c r="B8" s="9" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="D8" s="10"/>
     </row>
     <row r="9">
       <c r="B9" s="9" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10">
       <c r="B10" s="9" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="D10" s="10"/>
     </row>
     <row r="11">
       <c r="B11" s="9" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="9" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="D12" s="10"/>
     </row>
@@ -3433,32 +3850,32 @@
     </row>
     <row r="15">
       <c r="B15" s="7" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="11" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="11" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="11" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="11" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="11" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
     </row>
     <row r="24">
@@ -3559,120 +3976,120 @@
       <c r="B34" s="11"/>
     </row>
     <row r="36">
-      <c r="B36" s="45" t="s">
+      <c r="B36" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="46"/>
-      <c r="D36" s="46"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
     </row>
     <row r="37">
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="38" t="s">
+      <c r="C37" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="38" t="s">
+      <c r="D37" s="43" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="38">
-      <c r="B38" s="39" t="s">
-        <v>243</v>
-      </c>
-      <c r="C38" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" s="39" t="s">
-        <v>244</v>
+      <c r="B38" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="C38" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="44" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="39">
-      <c r="B39" s="39" t="s">
-        <v>245</v>
-      </c>
-      <c r="C39" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D39" s="39" t="s">
-        <v>246</v>
+      <c r="B39" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="C39" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="44" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="40">
-      <c r="B40" s="39" t="s">
-        <v>247</v>
-      </c>
-      <c r="C40" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D40" s="39" t="s">
-        <v>248</v>
+      <c r="B40" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="C40" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="44" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="41">
-      <c r="B41" s="39" t="s">
-        <v>249</v>
-      </c>
-      <c r="C41" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="D41" s="39" t="s">
-        <v>250</v>
+      <c r="B41" s="44" t="s">
+        <v>259</v>
+      </c>
+      <c r="C41" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="44" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" s="9" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" s="9" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" s="9" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" s="9" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" s="9" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="47">
@@ -3686,6 +4103,7 @@
       <c r="D48" s="16"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Phantom Knight 程式規格書.xlsx alpha 1.4 - Phantom Knight 美術、音樂、音效規格書.xlsx alpha 1.1
</commit_message>
<xml_diff>
--- a/企劃/Phantom Knight 程式規格書.xlsx
+++ b/企劃/Phantom Knight 程式規格書.xlsx
@@ -31,6 +31,22 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="C43">
+      <text>
+        <t xml:space="preserve">想到未來的倒數計時模式
+	-Henry Kuh</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
     <comment authorId="0" ref="B61">
       <text>
         <t xml:space="preserve">可多加一列『按鍵方法』
@@ -57,7 +73,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -76,7 +92,25 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="C4">
+      <text>
+        <t xml:space="preserve">離題）金靂：砍死戰象也只加一！
+	-Henry Kuh
+XDD
+	-Bridge Lin</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -105,7 +139,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -124,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="488">
   <si>
     <t>需求</t>
   </si>
@@ -190,6 +224,12 @@
   </si>
   <si>
     <t>新增戰鬥介面、系統、音樂音效的控制、遊戲暫停。修改操作分頁。</t>
+  </si>
+  <si>
+    <t>Alpha1.4</t>
+  </si>
+  <si>
+    <t>修改戰鬥介面</t>
   </si>
   <si>
     <t>概要</t>
@@ -1044,7 +1084,7 @@
     <t>戰鬥介面示意圖：</t>
   </si>
   <si>
-    <t>1.左下角放玩家頭像、血條、技能與其操作鍵位</t>
+    <t>1.左下角放玩家頭像、血條、狀態</t>
   </si>
   <si>
     <t>2. 用漫畫的打擊字取代傷害數字</t>
@@ -1074,10 +1114,31 @@
     <t>退到現在血量為止</t>
   </si>
   <si>
+    <t>1-2 頭像</t>
+  </si>
+  <si>
+    <t>跟著剩餘血量顯示不同的動畫</t>
+  </si>
+  <si>
+    <t>例如：血量50-100%神采奕奕的呼吸、30-50%咬牙、30%以下流汗喘息</t>
+  </si>
+  <si>
+    <t>1-3 狀態(三級製作目標)</t>
+  </si>
+  <si>
+    <t>顯示玩家身上的狀態</t>
+  </si>
+  <si>
+    <t>有狀態的時候才會顯示，無狀態時會隱藏</t>
+  </si>
+  <si>
+    <t>滑鼠hover時，顯示tooltip，告訴玩家這個狀態的功能</t>
+  </si>
+  <si>
     <t>2-1 傷害文字：</t>
   </si>
   <si>
-    <t>每一段有不同文字</t>
+    <t>每一段有不同文字(踩到敵人頭上也有相對應的)</t>
   </si>
   <si>
     <t>類似血咒之城的三剎斬：</t>
@@ -1116,7 +1177,11 @@
     <t>跳數字的時候震動</t>
   </si>
   <si>
-    <t>每10連擊(暫定)會有一個動畫</t>
+    <t>目前規劃：
+。10連-橘色火焰
+。30連-紅色火焰
+。50連-藍色火焰
+。100連-金色火焰</t>
   </si>
   <si>
     <t>5-1 分數：</t>
@@ -1149,10 +1214,13 @@
     <t>依照實際受到的傷害，與血量更新UI顯示</t>
   </si>
   <si>
-    <t>技能鍵位</t>
-  </si>
-  <si>
-    <t>依照現在技能的鍵位，UI上顯示</t>
+    <t>播放頭像動畫</t>
+  </si>
+  <si>
+    <t>依照血量播放對應的頭像動畫</t>
+  </si>
+  <si>
+    <t>顯示現在玩家身上的狀態</t>
   </si>
   <si>
     <t>傷害文字</t>
@@ -1189,6 +1257,15 @@
   </si>
   <si>
     <t>剩餘幾秒，計時器字體會變紅</t>
+  </si>
+  <si>
+    <t>狀態的功能</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>每個狀態的提示</t>
   </si>
   <si>
     <t>系統</t>
@@ -1625,11 +1702,6 @@
       <color rgb="FF0000FF"/>
     </font>
     <font>
-      <b/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <u/>
       <color rgb="FF1155CC"/>
     </font>
@@ -1662,6 +1734,11 @@
     <font>
       <u/>
       <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color rgb="FF000000"/>
@@ -1871,35 +1948,35 @@
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -1923,7 +2000,7 @@
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1983,7 +2060,7 @@
     <xdr:ext cx="1952625" cy="219075"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="圖片"/>
+        <xdr:cNvPr id="0" name="image12.png" title="圖片"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2011,7 +2088,7 @@
     <xdr:ext cx="1952625" cy="219075"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="圖片"/>
+        <xdr:cNvPr id="0" name="image5.png" title="圖片"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2039,7 +2116,7 @@
     <xdr:ext cx="1952625" cy="219075"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="圖片"/>
+        <xdr:cNvPr id="0" name="image6.png" title="圖片"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2067,7 +2144,7 @@
     <xdr:ext cx="1952625" cy="219075"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="圖片"/>
+        <xdr:cNvPr id="0" name="image4.png" title="圖片"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2089,13 +2166,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1981200" cy="219075"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="圖片"/>
+        <xdr:cNvPr id="0" name="image8.png" title="圖片"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2115,15 +2192,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>923925</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2943225" cy="1685925"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image13.png" title="圖片"/>
+        <xdr:cNvPr id="0" name="image14.png" title="圖片"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2156,7 +2233,7 @@
     <xdr:ext cx="9201150" cy="5419725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image14.png" title="圖片"/>
+        <xdr:cNvPr id="0" name="image13.png" title="圖片"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2213,7 +2290,7 @@
     <xdr:ext cx="4400550" cy="2476500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="圖片"/>
+        <xdr:cNvPr id="0" name="image7.png" title="圖片"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2241,7 +2318,7 @@
     <xdr:ext cx="2733675" cy="5105400"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.png" title="圖片"/>
+        <xdr:cNvPr id="0" name="image3.png" title="圖片"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2269,7 +2346,7 @@
     <xdr:ext cx="2076450" cy="6457950"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.png" title="圖片"/>
+        <xdr:cNvPr id="0" name="image10.png" title="圖片"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2310,7 +2387,7 @@
     <xdr:ext cx="1933575" cy="6362700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="圖片"/>
+        <xdr:cNvPr id="0" name="image11.png" title="圖片"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2338,7 +2415,7 @@
     <xdr:ext cx="4495800" cy="1247775"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.png" title="圖片"/>
+        <xdr:cNvPr id="0" name="image1.png" title="圖片"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2363,10 +2440,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2971800</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>-161925</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3467100" cy="4695825"/>
     <xdr:pic>
@@ -2432,7 +2509,7 @@
     <xdr:ext cx="4400550" cy="2476500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="圖片"/>
+        <xdr:cNvPr id="0" name="image7.png" title="圖片"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2880,7 +2957,7 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2909,40 +2986,40 @@
     </row>
     <row r="3">
       <c r="B3" s="10" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="8" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="8" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6">
       <c r="B6" s="8" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="8" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12">
@@ -3000,25 +3077,25 @@
     </row>
     <row r="15">
       <c r="B15" s="8" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E15" s="9"/>
     </row>
     <row r="16">
       <c r="B16" s="8" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="17">
@@ -3060,13 +3137,13 @@
       </c>
     </row>
     <row r="25">
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="38" t="s">
+      <c r="D25" s="37" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3116,7 +3193,8 @@
       <c r="D34" s="55"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3131,7 +3209,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="5.43"/>
-    <col customWidth="1" min="2" max="2" width="15.71"/>
+    <col customWidth="1" min="2" max="2" width="24.86"/>
     <col customWidth="1" min="3" max="3" width="54.0"/>
     <col customWidth="1" min="4" max="4" width="49.71"/>
     <col customWidth="1" min="5" max="5" width="43.29"/>
@@ -3140,7 +3218,7 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3169,7 +3247,7 @@
     </row>
     <row r="3">
       <c r="C3" s="6" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D3" s="6"/>
     </row>
@@ -3179,381 +3257,428 @@
     </row>
     <row r="13">
       <c r="C13" s="57" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="14">
       <c r="C14" s="57" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="15">
       <c r="C15" s="24" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16">
       <c r="C16" s="57" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="17">
       <c r="C17" s="10" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="19">
       <c r="C19" s="6" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20">
       <c r="C20" s="10" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="22">
       <c r="C22" s="10" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="24">
       <c r="C24" s="10" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="26">
       <c r="C26" s="10" t="s">
-        <v>308</v>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" s="43" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="30">
-      <c r="C30" s="6" t="s">
-        <v>309</v>
+      <c r="C30" s="40" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="31">
-      <c r="C31" s="10" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="C32" s="10" t="s">
-        <v>311</v>
+      <c r="C31" s="40" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="33">
       <c r="C33" s="43" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="34">
-      <c r="C34" s="10" t="s">
-        <v>313</v>
+      <c r="C34" s="40" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="C35" s="40" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="36">
-      <c r="C36" s="6" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="C37" s="10" t="s">
-        <v>315</v>
+      <c r="C36" s="40" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="38">
-      <c r="C38" s="10" t="s">
-        <v>316</v>
+      <c r="C38" s="6" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="39">
       <c r="C39" s="10" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="40">
       <c r="C40" s="10" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="41">
-      <c r="C41" s="10" t="s">
-        <v>319</v>
+      <c r="C41" s="42" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="C42" s="10" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="C44" s="6" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="45">
-      <c r="C45" s="6" t="s">
-        <v>320</v>
+      <c r="C45" s="10" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="46">
       <c r="C46" s="10" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="47">
       <c r="C47" s="10" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
     </row>
     <row r="48">
       <c r="C48" s="10" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="C50" s="6" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="C51" s="10" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="C52" s="32" t="s">
-        <v>326</v>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="C49" s="10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="C53" s="6" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="54">
-      <c r="C54" s="6" t="s">
-        <v>327</v>
+      <c r="C54" s="10" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="55">
       <c r="C55" s="10" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="56">
-      <c r="C56" s="10" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="C57" s="10" t="s">
-        <v>330</v>
+      <c r="C56" s="41" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="58">
-      <c r="C58" s="10" t="s">
-        <v>331</v>
+      <c r="C58" s="6" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="C59" s="10" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="60">
-      <c r="C60" s="10"/>
-    </row>
-    <row r="61">
-      <c r="A61" s="1"/>
-      <c r="B61" s="2" t="s">
+      <c r="C60" s="31" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="C62" s="6" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="C63" s="10" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="C64" s="10" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="C65" s="10" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="C66" s="10" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="C68" s="10"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="1"/>
+      <c r="B69" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
-      <c r="K61" s="4"/>
-      <c r="L61" s="4"/>
-      <c r="M61" s="4"/>
-      <c r="N61" s="4"/>
-      <c r="O61" s="4"/>
-      <c r="P61" s="4"/>
-      <c r="Q61" s="4"/>
-      <c r="R61" s="4"/>
-      <c r="S61" s="4"/>
-      <c r="T61" s="4"/>
-      <c r="U61" s="4"/>
-      <c r="V61" s="4"/>
-      <c r="W61" s="4"/>
-      <c r="X61" s="4"/>
-      <c r="Y61" s="4"/>
-      <c r="Z61" s="4"/>
-    </row>
-    <row r="62">
-      <c r="A62" s="5"/>
-      <c r="B62" s="6" t="s">
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="4"/>
+      <c r="N69" s="4"/>
+      <c r="O69" s="4"/>
+      <c r="P69" s="4"/>
+      <c r="Q69" s="4"/>
+      <c r="R69" s="4"/>
+      <c r="S69" s="4"/>
+      <c r="T69" s="4"/>
+      <c r="U69" s="4"/>
+      <c r="V69" s="4"/>
+      <c r="W69" s="4"/>
+      <c r="X69" s="4"/>
+      <c r="Y69" s="4"/>
+      <c r="Z69" s="4"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="5"/>
+      <c r="B70" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-    </row>
-    <row r="63">
-      <c r="B63" s="7" t="s">
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+    </row>
+    <row r="71">
+      <c r="B71" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C71" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D71" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="E71" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="64">
-      <c r="B64" s="8" t="s">
-        <v>332</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="D64" s="8"/>
-      <c r="E64" s="9"/>
-    </row>
-    <row r="65">
-      <c r="B65" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="D65" s="8"/>
-    </row>
-    <row r="66">
-      <c r="B66" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="D66" s="9"/>
-      <c r="E66" s="58" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="B67" s="8" t="s">
-        <v>338</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>315</v>
-      </c>
-      <c r="D67" s="8"/>
-      <c r="E67" s="9"/>
-    </row>
-    <row r="68">
-      <c r="B68" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-    </row>
-    <row r="69">
-      <c r="B69" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="C69" s="8" t="s">
+    <row r="72">
+      <c r="B72" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="D69" s="9"/>
-      <c r="E69" s="9"/>
-    </row>
-    <row r="70">
-      <c r="B70" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C70" s="8" t="s">
+      <c r="C72" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
-    </row>
-    <row r="71">
-      <c r="B71" s="10"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="9"/>
     </row>
     <row r="73">
-      <c r="B73" s="6" t="s">
+      <c r="B73" s="51" t="s">
+        <v>343</v>
+      </c>
+      <c r="C73" s="51" t="s">
+        <v>344</v>
+      </c>
+      <c r="D73" s="8"/>
+      <c r="E73" s="9"/>
+    </row>
+    <row r="74">
+      <c r="B74" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="C74" s="51" t="s">
+        <v>345</v>
+      </c>
+      <c r="D74" s="8"/>
+      <c r="E74" s="9"/>
+    </row>
+    <row r="75">
+      <c r="B75" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="D75" s="9"/>
+      <c r="E75" s="58" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="D76" s="8"/>
+      <c r="E76" s="9"/>
+    </row>
+    <row r="77">
+      <c r="B77" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+    </row>
+    <row r="78">
+      <c r="B78" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+    </row>
+    <row r="79">
+      <c r="B79" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+    </row>
+    <row r="80">
+      <c r="B80" s="10"/>
+    </row>
+    <row r="82">
+      <c r="B82" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="74">
-      <c r="B74" s="11" t="s">
+    <row r="83">
+      <c r="B83" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C74" s="12" t="s">
+      <c r="C83" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D74" s="12" t="s">
+      <c r="D83" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="75">
-      <c r="B75" s="17" t="s">
-        <v>343</v>
-      </c>
-      <c r="C75" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D75" s="17" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="B76" s="17" t="s">
-        <v>345</v>
-      </c>
-      <c r="C76" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D76" s="14"/>
-    </row>
-    <row r="77">
-      <c r="B77" s="15" t="s">
-        <v>346</v>
-      </c>
-      <c r="C77" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="D77" s="15" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="B78" s="15"/>
-      <c r="C78" s="15"/>
-      <c r="D78" s="16"/>
-    </row>
-    <row r="79">
-      <c r="B79" s="15"/>
-      <c r="C79" s="15"/>
-      <c r="D79" s="16"/>
-    </row>
-    <row r="80">
-      <c r="B80" s="15"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="16"/>
-    </row>
-    <row r="81">
-      <c r="B81" s="15"/>
-      <c r="C81" s="15"/>
-      <c r="D81" s="16"/>
-    </row>
-    <row r="82">
-      <c r="B82" s="15"/>
-      <c r="C82" s="15"/>
-      <c r="D82" s="16"/>
-    </row>
-    <row r="83">
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
-      <c r="D83" s="17"/>
+    <row r="84">
+      <c r="B84" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="C84" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D84" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="C85" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D85" s="14"/>
+    </row>
+    <row r="86">
+      <c r="B86" s="15" t="s">
+        <v>356</v>
+      </c>
+      <c r="C86" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D86" s="15" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="B87" s="52" t="s">
+        <v>358</v>
+      </c>
+      <c r="C87" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="D87" s="52" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" s="15"/>
+      <c r="C88" s="15"/>
+      <c r="D88" s="16"/>
+    </row>
+    <row r="89">
+      <c r="B89" s="15"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="16"/>
+    </row>
+    <row r="90">
+      <c r="B90" s="15"/>
+      <c r="C90" s="15"/>
+      <c r="D90" s="16"/>
+    </row>
+    <row r="91">
+      <c r="B91" s="13"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C33"/>
-    <hyperlink display="即時計算擊破數與連擊數的分數，詳見分數計算分頁" location="分數計算!A1" ref="C52"/>
-    <hyperlink r:id="rId2" ref="E66"/>
+    <hyperlink r:id="rId1" ref="C41"/>
+    <hyperlink display="即時計算擊破數與連擊數的分數，詳見分數計算分頁" location="分數計算!A1" ref="C60"/>
+    <hyperlink r:id="rId2" ref="E75"/>
   </hyperlinks>
   <drawing r:id="rId3"/>
 </worksheet>
@@ -3579,7 +3704,7 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>348</v>
+        <v>361</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3608,15 +3733,15 @@
     </row>
     <row r="3">
       <c r="B3" s="6" t="s">
-        <v>349</v>
-      </c>
-      <c r="C3" s="43" t="s">
-        <v>76</v>
+        <v>362</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="41" t="s">
-        <v>350</v>
+      <c r="B4" s="40" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="5">
@@ -3625,8 +3750,8 @@
       <c r="D5" s="3"/>
     </row>
     <row r="36">
-      <c r="B36" s="41" t="s">
-        <v>351</v>
+      <c r="B36" s="40" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="45">
@@ -3684,7 +3809,7 @@
     </row>
     <row r="48">
       <c r="B48" s="8" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
@@ -3817,7 +3942,7 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>353</v>
+        <v>366</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3846,24 +3971,24 @@
     </row>
     <row r="3">
       <c r="B3" s="6" t="s">
-        <v>354</v>
+        <v>367</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="10" t="s">
-        <v>355</v>
+        <v>368</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="10" t="s">
-        <v>356</v>
+        <v>369</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6">
       <c r="B6" s="10" t="s">
-        <v>357</v>
+        <v>370</v>
       </c>
     </row>
     <row r="18">
@@ -3921,7 +4046,7 @@
     </row>
     <row r="21">
       <c r="B21" s="8" t="s">
-        <v>358</v>
+        <v>371</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -3929,27 +4054,27 @@
     </row>
     <row r="22">
       <c r="B22" s="8" t="s">
-        <v>359</v>
+        <v>372</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
     <row r="23">
       <c r="B23" s="8" t="s">
-        <v>360</v>
+        <v>373</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>361</v>
+        <v>374</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
     </row>
     <row r="24">
       <c r="B24" s="8" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="9"/>
@@ -4061,7 +4186,7 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4090,7 +4215,7 @@
     </row>
     <row r="3">
       <c r="B3" s="10" t="s">
-        <v>365</v>
+        <v>378</v>
       </c>
     </row>
     <row r="4">
@@ -4098,34 +4223,34 @@
     </row>
     <row r="5">
       <c r="B5" s="6" t="s">
-        <v>366</v>
+        <v>379</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="10" t="s">
-        <v>367</v>
+        <v>380</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7">
       <c r="B7" s="10" t="s">
-        <v>368</v>
+        <v>381</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="6" t="s">
-        <v>369</v>
+        <v>382</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="10" t="s">
-        <v>370</v>
+        <v>383</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="10" t="s">
-        <v>371</v>
+        <v>384</v>
       </c>
     </row>
     <row r="20">
@@ -4183,20 +4308,20 @@
     </row>
     <row r="23">
       <c r="B23" s="8" t="s">
-        <v>372</v>
+        <v>385</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>373</v>
+        <v>386</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="9"/>
     </row>
     <row r="24">
       <c r="B24" s="8" t="s">
-        <v>374</v>
+        <v>387</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>375</v>
+        <v>388</v>
       </c>
       <c r="D24" s="8"/>
     </row>
@@ -4318,8 +4443,8 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="1"/>
-      <c r="B2" s="34" t="s">
-        <v>376</v>
+      <c r="B2" s="33" t="s">
+        <v>389</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4351,206 +4476,206 @@
     </row>
     <row r="4">
       <c r="B4" s="6" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="40" t="s">
-        <v>377</v>
+      <c r="C5" s="39" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>378</v>
+        <v>391</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7">
       <c r="B7" s="8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>379</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="8" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>381</v>
+        <v>394</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="8" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>383</v>
+        <v>396</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="8" t="s">
-        <v>384</v>
+        <v>397</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>385</v>
+        <v>398</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="8" t="s">
-        <v>386</v>
+        <v>399</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="8" t="s">
-        <v>388</v>
+        <v>401</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>389</v>
+        <v>402</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="8" t="s">
-        <v>390</v>
+        <v>403</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>391</v>
+        <v>404</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="8" t="s">
-        <v>392</v>
+        <v>405</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>393</v>
+        <v>406</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="8" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>394</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="8" t="s">
-        <v>395</v>
+        <v>408</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>396</v>
+        <v>409</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="8" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>397</v>
+        <v>410</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="8" t="s">
-        <v>398</v>
+        <v>411</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>399</v>
+        <v>412</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="6" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>400</v>
+        <v>413</v>
       </c>
       <c r="D21" s="27"/>
     </row>
     <row r="22">
       <c r="B22" s="8" t="s">
-        <v>401</v>
+        <v>414</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>402</v>
+        <v>415</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>403</v>
+        <v>416</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" s="8" t="s">
-        <v>404</v>
+        <v>417</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>405</v>
+        <v>418</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>406</v>
+        <v>419</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="8" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>408</v>
+        <v>421</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>409</v>
+        <v>422</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" s="8" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>411</v>
+        <v>424</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>412</v>
+        <v>425</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="8" t="s">
-        <v>413</v>
+        <v>426</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>414</v>
+        <v>427</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>415</v>
+        <v>428</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" s="8" t="s">
-        <v>416</v>
+        <v>429</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" s="8" t="s">
-        <v>419</v>
+        <v>432</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>420</v>
+        <v>433</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>421</v>
+        <v>434</v>
       </c>
     </row>
     <row r="31">
@@ -4656,113 +4781,113 @@
       </c>
     </row>
     <row r="44">
-      <c r="B44" s="37" t="s">
+      <c r="B44" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="38" t="s">
+      <c r="C44" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D44" s="38" t="s">
+      <c r="D44" s="37" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" s="59" t="s">
-        <v>422</v>
+        <v>435</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" s="59" t="s">
-        <v>423</v>
+        <v>436</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" s="17" t="s">
-        <v>424</v>
+        <v>437</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" s="17" t="s">
-        <v>425</v>
+        <v>438</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" s="17" t="s">
-        <v>426</v>
+        <v>439</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" s="59" t="s">
-        <v>427</v>
+        <v>440</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" s="59" t="s">
-        <v>428</v>
+        <v>441</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" s="59" t="s">
-        <v>429</v>
+        <v>442</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" s="59" t="s">
-        <v>430</v>
+        <v>443</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -4790,8 +4915,8 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="1"/>
-      <c r="B2" s="34" t="s">
-        <v>431</v>
+      <c r="B2" s="33" t="s">
+        <v>444</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4820,85 +4945,85 @@
     </row>
     <row r="4">
       <c r="B4" s="6" t="s">
-        <v>432</v>
+        <v>445</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>433</v>
+        <v>446</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="8" t="s">
-        <v>434</v>
+        <v>447</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>435</v>
+        <v>448</v>
       </c>
       <c r="D5" s="60"/>
     </row>
     <row r="6">
       <c r="B6" s="8" t="s">
-        <v>436</v>
+        <v>449</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>438</v>
+        <v>451</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="8" t="s">
-        <v>439</v>
+        <v>452</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>440</v>
+        <v>453</v>
       </c>
       <c r="D7" s="9"/>
     </row>
     <row r="8">
       <c r="B8" s="8" t="s">
-        <v>441</v>
+        <v>454</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>442</v>
+        <v>455</v>
       </c>
       <c r="D8" s="9"/>
     </row>
     <row r="9">
       <c r="B9" s="8" t="s">
-        <v>443</v>
+        <v>456</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>444</v>
+        <v>457</v>
       </c>
       <c r="D9" s="9"/>
     </row>
     <row r="10">
       <c r="B10" s="8" t="s">
-        <v>445</v>
+        <v>458</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="D10" s="9"/>
     </row>
     <row r="11">
       <c r="B11" s="8" t="s">
-        <v>447</v>
+        <v>460</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>448</v>
+        <v>461</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>449</v>
+        <v>462</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="8" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
       <c r="D12" s="9"/>
     </row>
@@ -4909,32 +5034,32 @@
     </row>
     <row r="15">
       <c r="B15" s="6" t="s">
-        <v>452</v>
+        <v>465</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="10" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="10" t="s">
-        <v>454</v>
+        <v>467</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="10" t="s">
-        <v>455</v>
+        <v>468</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="10" t="s">
-        <v>456</v>
+        <v>469</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="10" t="s">
-        <v>457</v>
+        <v>470</v>
       </c>
     </row>
     <row r="24">
@@ -5054,101 +5179,101 @@
     </row>
     <row r="38">
       <c r="B38" s="17" t="s">
-        <v>458</v>
+        <v>471</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>459</v>
+        <v>472</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" s="17" t="s">
-        <v>460</v>
+        <v>473</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>461</v>
+        <v>474</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" s="17" t="s">
-        <v>462</v>
+        <v>475</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>463</v>
+        <v>476</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" s="17" t="s">
-        <v>464</v>
+        <v>477</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>465</v>
+        <v>478</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" s="8" t="s">
-        <v>466</v>
+        <v>479</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>467</v>
+        <v>480</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" s="8" t="s">
-        <v>468</v>
+        <v>481</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>469</v>
+        <v>482</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" s="8" t="s">
-        <v>470</v>
+        <v>483</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" s="8" t="s">
-        <v>471</v>
+        <v>484</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>472</v>
+        <v>485</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" s="8" t="s">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>474</v>
+        <v>487</v>
       </c>
     </row>
     <row r="47">
@@ -5250,6 +5375,20 @@
         <v>21</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="20">
+        <v>44642.0</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -5271,7 +5410,7 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -5300,7 +5439,7 @@
     </row>
     <row r="3">
       <c r="B3" s="23" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C3" s="24"/>
     </row>
@@ -5310,50 +5449,50 @@
     </row>
     <row r="5">
       <c r="B5" s="26" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="28" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="28" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="28" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="28" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="28" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11">
@@ -5361,42 +5500,42 @@
     </row>
     <row r="12">
       <c r="B12" s="28" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="28" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="28" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="28" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="28" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17">
@@ -5405,101 +5544,101 @@
     </row>
     <row r="18">
       <c r="B18" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="6"/>
-      <c r="C19" s="31" t="s">
-        <v>47</v>
+      <c r="C19" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="20">
-      <c r="C20" s="32" t="s">
-        <v>48</v>
+      <c r="C20" s="31" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21">
-      <c r="C21" s="32" t="s">
-        <v>49</v>
+      <c r="C21" s="31" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="22">
-      <c r="C22" s="32" t="s">
-        <v>50</v>
+      <c r="C22" s="31" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="23">
-      <c r="C23" s="32" t="s">
-        <v>51</v>
+      <c r="C23" s="31" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="24">
-      <c r="C24" s="32" t="s">
-        <v>52</v>
+      <c r="C24" s="31" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="25">
-      <c r="C25" s="32" t="s">
-        <v>53</v>
+      <c r="C25" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="26">
-      <c r="C26" s="32" t="s">
-        <v>54</v>
+      <c r="C26" s="31" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="27">
-      <c r="C27" s="32" t="s">
-        <v>55</v>
+      <c r="C27" s="31" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="28">
-      <c r="C28" s="32" t="s">
-        <v>56</v>
+      <c r="C28" s="31" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="29">
-      <c r="C29" s="32" t="s">
-        <v>57</v>
+      <c r="C29" s="31" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="30">
-      <c r="C30" s="32" t="s">
-        <v>58</v>
+      <c r="C30" s="31" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="31">
       <c r="C31" s="6"/>
     </row>
     <row r="32">
-      <c r="C32" s="31" t="s">
-        <v>59</v>
+      <c r="C32" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="33">
-      <c r="C33" s="33" t="s">
-        <v>60</v>
+      <c r="C33" s="32" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="34">
-      <c r="C34" s="32" t="s">
-        <v>61</v>
+      <c r="C34" s="31" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="35">
       <c r="C35" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36">
       <c r="C36" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37">
       <c r="C37" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -5543,8 +5682,8 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="1"/>
-      <c r="B2" s="34" t="s">
-        <v>65</v>
+      <c r="B2" s="33" t="s">
+        <v>67</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -5573,28 +5712,28 @@
     </row>
     <row r="3">
       <c r="B3" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D3" s="10"/>
     </row>
     <row r="4">
       <c r="B4" s="10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8">
@@ -5605,47 +5744,47 @@
     </row>
     <row r="10">
       <c r="B10" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" s="10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" s="10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="35" t="s">
-        <v>75</v>
+      <c r="B32" s="34" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="33">
-      <c r="B33" s="36" t="s">
-        <v>76</v>
+      <c r="B33" s="35" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="38">
@@ -5724,34 +5863,34 @@
     </row>
     <row r="41">
       <c r="B41" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E41" s="9"/>
     </row>
     <row r="42">
       <c r="B42" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E42" s="9"/>
     </row>
     <row r="43">
       <c r="B43" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
@@ -5774,47 +5913,47 @@
       </c>
     </row>
     <row r="48">
-      <c r="B48" s="37" t="s">
+      <c r="B48" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="38" t="s">
+      <c r="C48" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="38" t="s">
+      <c r="D48" s="37" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C50" s="8" t="s">
-        <v>86</v>
-      </c>
       <c r="D50" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52">
@@ -5829,9 +5968,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" location="G198RaeA3XA_b2Xfwl_2D2yFxYfitIzsvj" ref="B33"/>
+    <hyperlink r:id="rId2" location="G198RaeA3XA_b2Xfwl_2D2yFxYfitIzsvj" ref="B33"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -5854,8 +5994,8 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="1"/>
-      <c r="B2" s="34" t="s">
-        <v>93</v>
+      <c r="B2" s="33" t="s">
+        <v>95</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -5884,93 +6024,93 @@
     </row>
     <row r="3">
       <c r="B3" s="10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="39" t="s">
-        <v>95</v>
+      <c r="B4" s="38" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" s="40" t="s">
+      <c r="B6" s="39" t="s">
         <v>98</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16">
@@ -5981,214 +6121,214 @@
     </row>
     <row r="18">
       <c r="B18" s="6" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="10" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="10" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="41" t="s">
-        <v>119</v>
+      <c r="B22" s="40" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" s="10" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" s="6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="10" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" s="10" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="D28" s="43" t="s">
-        <v>124</v>
+      <c r="B28" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" s="6" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" s="10" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" s="10" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" s="10" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" s="10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" s="10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" s="10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" s="10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" s="10" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" s="10" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" s="10" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" s="10" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" s="10"/>
     </row>
     <row r="48">
-      <c r="B48" s="32" t="s">
-        <v>139</v>
+      <c r="B48" s="31" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="51">
-      <c r="B51" s="31" t="s">
-        <v>140</v>
+      <c r="B51" s="43" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="52">
-      <c r="B52" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="C52" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="D52" s="40" t="s">
+      <c r="B52" s="39" t="s">
         <v>98</v>
+      </c>
+      <c r="C52" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="D52" s="39" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" s="8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" s="8" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" s="8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" s="8" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="59">
@@ -6247,10 +6387,10 @@
     <row r="62">
       <c r="A62" s="44"/>
       <c r="B62" s="45" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C62" s="45" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D62" s="46"/>
       <c r="E62" s="46"/>
@@ -6278,78 +6418,78 @@
     </row>
     <row r="63">
       <c r="B63" s="8" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E63" s="9"/>
     </row>
     <row r="64">
       <c r="B64" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="E64" s="43" t="s">
-        <v>124</v>
+        <v>160</v>
+      </c>
+      <c r="E64" s="42" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" s="8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
     </row>
     <row r="66">
       <c r="B66" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E66" s="9"/>
     </row>
     <row r="67">
       <c r="B67" s="8" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
     </row>
     <row r="68">
       <c r="B68" s="8" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
     </row>
     <row r="69">
       <c r="B69" s="8" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
@@ -6375,80 +6515,80 @@
     </row>
     <row r="74">
       <c r="B74" s="13" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="75">
       <c r="B75" s="15" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="76">
       <c r="B76" s="15" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D76" s="16"/>
     </row>
     <row r="77">
       <c r="B77" s="15" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D77" s="16"/>
     </row>
     <row r="78">
       <c r="B78" s="15" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D78" s="16"/>
     </row>
     <row r="79">
       <c r="B79" s="15" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D79" s="16"/>
     </row>
     <row r="80">
       <c r="B80" s="15" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D80" s="16"/>
     </row>
     <row r="81">
       <c r="B81" s="13" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -6482,8 +6622,8 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="1"/>
-      <c r="B2" s="34" t="s">
-        <v>180</v>
+      <c r="B2" s="33" t="s">
+        <v>182</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -6512,160 +6652,160 @@
     </row>
     <row r="3">
       <c r="B3" s="10" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="41" t="s">
-        <v>182</v>
+      <c r="B4" s="40" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="41"/>
+      <c r="B5" s="40"/>
     </row>
     <row r="6">
       <c r="B6" s="6" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7">
       <c r="B7" s="8" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D7" s="9"/>
     </row>
     <row r="8">
       <c r="B8" s="8" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D8" s="9"/>
     </row>
     <row r="9">
       <c r="B9" s="8" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D9" s="9"/>
     </row>
     <row r="10">
       <c r="B10" s="8" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D10" s="9"/>
     </row>
     <row r="11">
       <c r="B11" s="8" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="8" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D12" s="9"/>
     </row>
     <row r="15">
       <c r="B15" s="6" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="21" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="49" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="8" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="8" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="8" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" s="8" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" s="8" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" s="6" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="8" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D26" s="9"/>
     </row>
@@ -6675,32 +6815,32 @@
       <c r="D27" s="10"/>
     </row>
     <row r="28">
-      <c r="B28" s="31" t="s">
-        <v>217</v>
-      </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
+      <c r="B28" s="43" t="s">
+        <v>219</v>
+      </c>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
     </row>
     <row r="29">
       <c r="B29" s="51" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D29" s="51" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="51" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D30" s="51" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32">
@@ -6758,10 +6898,10 @@
     </row>
     <row r="35">
       <c r="B35" s="8" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="9"/>
@@ -6822,139 +6962,139 @@
     </row>
     <row r="46">
       <c r="B46" s="17" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D46" s="13"/>
     </row>
     <row r="47">
       <c r="B47" s="17" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" s="17" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D49" s="17" t="s">
         <v>229</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" s="17" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" s="15" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D51" s="14"/>
     </row>
     <row r="52">
       <c r="B52" s="15" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D52" s="15"/>
     </row>
     <row r="53">
       <c r="B53" s="15" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" s="15" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" s="15" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" s="15" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" s="51" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C57" s="52" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D57" s="52" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" s="51" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C58" s="52" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D58" s="52" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="59">
@@ -7003,7 +7143,7 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -7032,10 +7172,10 @@
     </row>
     <row r="3">
       <c r="B3" s="6" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6">
@@ -7098,39 +7238,39 @@
     </row>
     <row r="40">
       <c r="B40" s="8" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="9"/>
     </row>
     <row r="41">
       <c r="B41" s="8" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D41" s="8"/>
     </row>
     <row r="42">
       <c r="B42" s="8" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
     </row>
     <row r="43">
       <c r="B43" s="8" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="9"/>
@@ -7162,13 +7302,13 @@
       </c>
     </row>
     <row r="50">
-      <c r="B50" s="37" t="s">
+      <c r="B50" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C50" s="38" t="s">
+      <c r="C50" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="38" t="s">
+      <c r="D50" s="37" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7242,7 +7382,7 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -7271,18 +7411,18 @@
     </row>
     <row r="3">
       <c r="B3" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="10" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5">
@@ -7292,167 +7432,167 @@
     </row>
     <row r="6">
       <c r="B6" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7">
       <c r="B7" s="8" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8">
       <c r="B8" s="8" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D8" s="3"/>
     </row>
     <row r="9">
       <c r="B9" s="8" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C9" s="56" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D9" s="3"/>
     </row>
     <row r="10">
       <c r="B10" s="8" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D10" s="3"/>
     </row>
     <row r="11">
       <c r="B11" s="8" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12">
       <c r="B12" s="8" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C12" s="56" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13">
       <c r="B13" s="8" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="10" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="41"/>
+      <c r="B14" s="40"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="10" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="6" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="8" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="8" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="8" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="8" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="8" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" s="6" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="8" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" s="8" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28">
@@ -7510,58 +7650,58 @@
     </row>
     <row r="31">
       <c r="B31" s="8" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="9"/>
     </row>
     <row r="32">
       <c r="B32" s="8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D32" s="8"/>
     </row>
     <row r="33">
       <c r="B33" s="8" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
     </row>
     <row r="34">
       <c r="B34" s="8" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="9"/>
     </row>
     <row r="35">
       <c r="B35" s="8" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="E35" s="9"/>
     </row>
     <row r="36">
       <c r="B36" s="8" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="9"/>
@@ -7582,13 +7722,13 @@
       </c>
     </row>
     <row r="41">
-      <c r="B41" s="37" t="s">
+      <c r="B41" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="38" t="s">
+      <c r="C41" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="38" t="s">
+      <c r="D41" s="37" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7662,7 +7802,7 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -7691,12 +7831,12 @@
     </row>
     <row r="3">
       <c r="B3" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="41" t="s">
-        <v>277</v>
+      <c r="B4" s="40" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="6">
@@ -7709,17 +7849,17 @@
     </row>
     <row r="18">
       <c r="B18" s="10" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="10" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="10" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="23">
@@ -7825,13 +7965,13 @@
       </c>
     </row>
     <row r="36">
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="38" t="s">
+      <c r="C36" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="38" t="s">
+      <c r="D36" s="37" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>